<commit_message>
20251217 AETAW fixed capping
</commit_message>
<xml_diff>
--- a/GUI + Reviews/202512/AEX Family.xlsx
+++ b/GUI + Reviews/202512/AEX Family.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="V:\PM-Indices-IndexOperations\Review Files\202512\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://euronext-my.sharepoint.com/personal/csonneveld_euronext_com/Documents/Documents/Projects/GUI + Reviews/202512/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF367D4E-A8F9-4415-AB96-3AC0CBDF2F5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{FF367D4E-A8F9-4415-AB96-3AC0CBDF2F5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9F95F698-5B4B-46C2-807C-2AFAACF2D151}"/>
   <bookViews>
-    <workbookView xWindow="-29370" yWindow="195" windowWidth="29040" windowHeight="15720" xr2:uid="{A63E6ABF-5363-4D23-86E3-0F726F43561F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{A63E6ABF-5363-4D23-86E3-0F726F43561F}"/>
   </bookViews>
   <sheets>
     <sheet name="AEX" sheetId="1" r:id="rId1"/>
@@ -758,6 +758,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1059,7 +1063,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B8F9A41-73C2-4E38-AC56-DEDEBD5758A5}">
   <dimension ref="A1:G32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
@@ -2467,8 +2471,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30E4D7D2-284F-49E6-B2E9-80ED5EB35E15}">
   <dimension ref="A1:G22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="44.5" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2872,7 +2876,7 @@
         <v>10</v>
       </c>
       <c r="D18" s="5">
-        <v>70000000</v>
+        <v>78750000</v>
       </c>
       <c r="E18" s="6">
         <v>0.35</v>

</xml_diff>